<commit_message>
Added sixth meeting minutes
</commit_message>
<xml_diff>
--- a/Alex/Cold Gas Thrusters/Cold Gas Thrusters.xlsx
+++ b/Alex/Cold Gas Thrusters/Cold Gas Thrusters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CubeSat_project\Alex\Cold Gas Thrusters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D975E0A-F9E2-478F-85FC-6EE8A6F962A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6ACFFD-6D5D-479C-8957-FB34D4238FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6B4DF1FC-0F25-411A-9333-4E58E79A1DAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B4DF1FC-0F25-411A-9333-4E58E79A1DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,29 +541,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE4C822-FAB6-4DDE-8446-94A137D4E186}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="24.85546875" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="45.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" customWidth="1"/>
+    <col min="12" max="12" width="24.88671875" customWidth="1"/>
+    <col min="14" max="14" width="20.88671875" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
     <col min="16" max="16" width="113" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -613,7 +613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -657,7 +657,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -693,7 +693,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>